<commit_message>
Commited on 13th Feb 2019
</commit_message>
<xml_diff>
--- a/Testing_Practice/Input/data.xlsx
+++ b/Testing_Practice/Input/data.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>naresh</t>
   </si>
   <si>
     <t>venu</t>
+  </si>
+  <si>
+    <t>ramu</t>
+  </si>
+  <si>
+    <t>ramu123</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,6 +381,14 @@
       </c>
       <c r="B2">
         <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>